<commit_message>
1. pinmux sheet corrected
</commit_message>
<xml_diff>
--- a/LR1121DVK1TBKS/Docs/pinmux.xlsx
+++ b/LR1121DVK1TBKS/Docs/pinmux.xlsx
@@ -687,15 +687,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
@@ -1222,7 +1222,7 @@
         <v>75</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="F41" s="7"/>
     </row>
@@ -1237,7 +1237,7 @@
         <v>78</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="F42" s="7"/>
     </row>
@@ -1252,7 +1252,7 @@
         <v>81</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F43" s="7"/>
     </row>
@@ -1267,7 +1267,7 @@
         <v>84</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F44" s="7"/>
     </row>
@@ -1282,7 +1282,7 @@
         <v>87</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F45" s="7"/>
     </row>
@@ -1297,7 +1297,7 @@
         <v>90</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="F46" s="7"/>
     </row>

</xml_diff>

<commit_message>
1. Corrected the SPI1 configuration for LR1121 chipset. Nuclo have option for SPI1 & SPI2, default is SPI1
</commit_message>
<xml_diff>
--- a/LR1121DVK1TBKS/Docs/pinmux.xlsx
+++ b/LR1121DVK1TBKS/Docs/pinmux.xlsx
@@ -84,9 +84,6 @@
     <t>D13</t>
   </si>
   <si>
-    <t>PB13</t>
-  </si>
-  <si>
     <t>LORA SPI LINES</t>
   </si>
   <si>
@@ -96,18 +93,12 @@
     <t>D12</t>
   </si>
   <si>
-    <t>PB14</t>
-  </si>
-  <si>
     <t>MOSI</t>
   </si>
   <si>
     <t>D11</t>
   </si>
   <si>
-    <t>PB15</t>
-  </si>
-  <si>
     <t>TFT_CS</t>
   </si>
   <si>
@@ -295,6 +286,15 @@
   </si>
   <si>
     <t>PC0</t>
+  </si>
+  <si>
+    <t>PA5</t>
+  </si>
+  <si>
+    <t>PA6</t>
+  </si>
+  <si>
+    <t>PA7</t>
   </si>
 </sst>
 </file>
@@ -388,23 +388,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,12 +709,12 @@
       <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -726,161 +726,161 @@
       <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>9</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>8</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="8" t="s">
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="5">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="5">
-        <v>4</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="E12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="5">
-        <v>3</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C17" s="2" t="s">
@@ -892,145 +892,145 @@
       <c r="E17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="9">
+      <c r="B19" s="6">
         <v>1</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="6">
+        <v>3</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="9">
-        <v>2</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="9">
-        <v>3</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="6">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="9">
-        <v>4</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B23" s="6">
+        <v>5</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="9">
-        <v>5</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" s="6">
+        <v>6</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="9">
-        <v>6</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="6">
+        <v>7</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D25" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E25" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="9">
-        <v>7</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" s="6">
+        <v>8</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E26" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="9">
-        <v>8</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
@@ -1043,144 +1043,144 @@
       <c r="E28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="9">
+      <c r="B30" s="6">
         <v>1</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="9">
+      <c r="B31" s="6">
         <v>2</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="9">
+      <c r="B32" s="6">
         <v>3</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B33" s="6">
+        <v>4</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="E33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B34" s="6">
+        <v>5</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B33" s="9">
-        <v>4</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="D34" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B35" s="6">
+        <v>6</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="6">
+        <v>7</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="6">
+        <v>8</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B34" s="9">
-        <v>5</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B35" s="9">
-        <v>6</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B36" s="9">
-        <v>7</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B37" s="9">
-        <v>8</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F37" s="10"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C39" s="2" t="s">
@@ -1192,123 +1192,123 @@
       <c r="E39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="6"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B41" s="9">
+      <c r="B41" s="6">
         <v>1</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="6">
+        <v>2</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D42" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F41" s="7"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B42" s="9">
-        <v>2</v>
-      </c>
-      <c r="C42" s="7" t="s">
+      <c r="E42" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B43" s="6">
+        <v>3</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D43" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E42" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B43" s="9">
-        <v>3</v>
-      </c>
-      <c r="C43" s="7" t="s">
+      <c r="E43" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B44" s="6">
+        <v>4</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B44" s="9">
-        <v>4</v>
-      </c>
-      <c r="C44" s="7" t="s">
+      <c r="E44" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B45" s="6">
+        <v>5</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D45" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B45" s="9">
-        <v>5</v>
-      </c>
-      <c r="C45" s="7" t="s">
+      <c r="E45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="6">
+        <v>6</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D46" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E45" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F45" s="7"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B46" s="9">
-        <v>6</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F46" s="7"/>
+      <c r="E46" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F46" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F39:F40"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F39:F40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>